<commit_message>
added new version (3.8.1)
</commit_message>
<xml_diff>
--- a/01_DataSources/DS_cleanVersion_TEST.xlsx
+++ b/01_DataSources/DS_cleanVersion_TEST.xlsx
@@ -1,33 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\soapuiplus-3.0\01_DataSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_WORK\01_Actual_work\01_CLV\01_Projects\01_CAT\01_Github\soapuiplus-3.0\01_DataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E975676-F0B2-459C-9663-74FAAD3A8499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="3828" yWindow="1848" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>tcId</t>
   </si>
@@ -44,32 +37,48 @@
     <t>testVariantDesc</t>
   </si>
   <si>
+    <t>dsVal2</t>
+  </si>
+  <si>
+    <t>dsVal3</t>
+  </si>
+  <si>
+    <t>testCase1</t>
+  </si>
+  <si>
+    <t>TC01TV01</t>
+  </si>
+  <si>
+    <t>varianta_1</t>
+  </si>
+  <si>
+    <t>xrayTestExecKey</t>
+  </si>
+  <si>
+    <t>xrayTestKey</t>
+  </si>
+  <si>
     <t>dsVal1</t>
   </si>
   <si>
-    <t>dsVal2</t>
-  </si>
-  <si>
-    <t>dsVal3</t>
-  </si>
-  <si>
-    <t>testCase1</t>
-  </si>
-  <si>
-    <t>TC01TV01</t>
-  </si>
-  <si>
-    <t>varianta_1</t>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -497,23 +506,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="3" width="16.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="19.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="7" width="19.5546875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="15.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,35 +540,47 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2"/>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>